<commit_message>
feat：update droppoint and sceneunit excel
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/DropPoint_资源生成点表.xlsx
+++ b/pet-simulator/Excel/DropPoint_资源生成点表.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -5181,6 +5181,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -5188,8 +5294,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1123" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1131" activeCellId="0" sqref="G1131"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1591" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1611" activeCellId="0" sqref="F1611"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24611,7 +24717,10 @@
         <v>1612</v>
       </c>
       <c r="C1607" s="15" t="n">
-        <v>3003</v>
+        <v>2007</v>
+      </c>
+      <c r="D1607" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1608" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24622,7 +24731,10 @@
         <v>1613</v>
       </c>
       <c r="C1608" s="15" t="n">
-        <v>3004</v>
+        <v>2008</v>
+      </c>
+      <c r="D1608" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1609" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24633,7 +24745,10 @@
         <v>1614</v>
       </c>
       <c r="C1609" s="15" t="n">
-        <v>3005</v>
+        <v>2009</v>
+      </c>
+      <c r="D1609" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1610" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24644,7 +24759,10 @@
         <v>1615</v>
       </c>
       <c r="C1610" s="15" t="n">
-        <v>3006</v>
+        <v>2010</v>
+      </c>
+      <c r="D1610" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1611" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat：fix world2 treasure bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/DropPoint_资源生成点表.xlsx
+++ b/pet-simulator/Excel/DropPoint_资源生成点表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="1554">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -3908,39 +3908,24 @@
     <t xml:space="preserve">-32525|123958|79629</t>
   </si>
   <si>
-    <t xml:space="preserve">2258.41|100302.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2582.41|100233.08|73139.95</t>
   </si>
   <si>
     <t xml:space="preserve">2479.41|100468.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2758.41|100109.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2623.41|99839.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2623.41|100651.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2894.41|99903.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2267.41|99829.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2190.41|100569.08|73139.95</t>
   </si>
   <si>
     <t xml:space="preserve">1526.41|100057.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">1664.41|100233.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">1803.41|100406.08|73139.95</t>
   </si>
   <si>
@@ -3950,9 +3935,6 @@
     <t xml:space="preserve">1705.41|99839.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">1705.41|100651.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">1349.41|99829.08|73139.95</t>
   </si>
   <si>
@@ -3962,18 +3944,12 @@
     <t xml:space="preserve">1272.41|100084.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">1733.41|99075.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">1547.41|99320.08|73139.95</t>
   </si>
   <si>
     <t xml:space="preserve">1871.41|99251.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2010.41|99424.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2218.41|99257.08|73139.95</t>
   </si>
   <si>
@@ -3983,9 +3959,6 @@
     <t xml:space="preserve">1912.41|99669.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2183.41|98921.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">1556.41|98847.08|73139.95</t>
   </si>
   <si>
@@ -3995,9 +3968,6 @@
     <t xml:space="preserve">2689.41|99075.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2503.41|99320.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2827.41|99251.08|73139.95</t>
   </si>
   <si>
@@ -4010,15 +3980,9 @@
     <t xml:space="preserve">3003.41|99127.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2868.41|98857.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2868.41|99669.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2512.41|98847.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2435.41|99587.08|73139.95</t>
   </si>
   <si>
@@ -4028,30 +3992,18 @@
     <t xml:space="preserve">2885.41|98113.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3023.41|98289.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2920.41|98524.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3162.41|98462.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3370.41|98295.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3064.41|97895.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3064.41|98707.08|73139.95</t>
   </si>
   <si>
     <t xml:space="preserve">3335.41|97959.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2631.41|98625.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2631.41|98140.08|73139.95</t>
   </si>
   <si>
@@ -4064,9 +4016,6 @@
     <t xml:space="preserve">1131.41|98642.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">1131.41|99012.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">2021.41|98524.08|73139.95</t>
   </si>
   <si>
@@ -4079,9 +4028,6 @@
     <t xml:space="preserve">2165.41|97895.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2436.41|97959.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">1809.41|97885.08|73139.95</t>
   </si>
   <si>
@@ -4091,9 +4037,6 @@
     <t xml:space="preserve">3810.41|98113.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3624.41|98358.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3845.41|98524.08|73139.95</t>
   </si>
   <si>
@@ -4103,9 +4046,6 @@
     <t xml:space="preserve">4295.41|98295.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3989.41|97895.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3989.41|98707.08|73139.95</t>
   </si>
   <si>
@@ -4118,15 +4058,9 @@
     <t xml:space="preserve">3556.41|98140.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3651.41|99084.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3789.41|99260.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3686.41|99495.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">4136.41|99266.08|73139.95</t>
   </si>
   <si>
@@ -4136,18 +4070,12 @@
     <t xml:space="preserve">3830.41|99678.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">4101.41|98930.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3397.41|99596.08|73139.95</t>
   </si>
   <si>
     <t xml:space="preserve">3397.41|99111.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3222.41|100313.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3546.41|100244.08|73139.95</t>
   </si>
   <si>
@@ -4157,9 +4085,6 @@
     <t xml:space="preserve">3722.41|100120.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3587.41|99850.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3587.41|100662.08|73139.95</t>
   </si>
   <si>
@@ -4184,9 +4109,6 @@
     <t xml:space="preserve">3074.41|101036.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">2888.41|101281.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3109.41|101447.08|73139.95</t>
   </si>
   <si>
@@ -4196,9 +4118,6 @@
     <t xml:space="preserve">3388.41|101088.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">3253.41|101630.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">3524.41|100882.08|73139.95</t>
   </si>
   <si>
@@ -4217,9 +4136,6 @@
     <t xml:space="preserve">4326.41|99332.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">4403.41|98592.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">5030.41|98666.08|73139.95</t>
   </si>
   <si>
@@ -4229,9 +4145,6 @@
     <t xml:space="preserve">4759.41|98602.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">5065.41|99002.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">4857.41|99169.08|73139.95</t>
   </si>
   <si>
@@ -4241,9 +4154,6 @@
     <t xml:space="preserve">4718.41|98996.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">4394.41|99065.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">4580.41|98820.08|73139.95</t>
   </si>
   <si>
@@ -4259,9 +4169,6 @@
     <t xml:space="preserve">4557.41|100564.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">4557.41|99752.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">4692.41|100022.08|73139.95</t>
   </si>
   <si>
@@ -4274,9 +4181,6 @@
     <t xml:space="preserve">5594.41|100540.08|73139.95</t>
   </si>
   <si>
-    <t xml:space="preserve">5238.41|100451.08|73139.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">4863.41|100152.08|73139.95</t>
   </si>
   <si>
@@ -4343,9 +4247,6 @@
     <t xml:space="preserve">-8583.59|84233.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8163.59|84233.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-8325.59|83454.08|77527.95</t>
   </si>
   <si>
@@ -4355,9 +4256,6 @@
     <t xml:space="preserve">-8168.59|82743.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7821.59|82743.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7556.59|82950.08|77527.95</t>
   </si>
   <si>
@@ -4367,9 +4265,6 @@
     <t xml:space="preserve">-8549.59|82743.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8708.59|83014.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-8583.59|83284.08|77527.95</t>
   </si>
   <si>
@@ -4379,9 +4274,6 @@
     <t xml:space="preserve">-7569.59|83903.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7273.59|83494.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7412.59|83192.08|77527.95</t>
   </si>
   <si>
@@ -4391,18 +4283,12 @@
     <t xml:space="preserve">-7827.59|83733.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7407.59|83733.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6677.59|84330.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-6677.59|83921.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6381.59|83921.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6901.59|83619.08|77527.95</t>
   </si>
   <si>
@@ -4412,9 +4298,6 @@
     <t xml:space="preserve">-6935.59|84160.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6677.59|83437.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6677.59|83028.08|77527.95</t>
   </si>
   <si>
@@ -4424,9 +4307,6 @@
     <t xml:space="preserve">-6520.59|82726.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6690.59|82461.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7060.59|82997.08|77527.95</t>
   </si>
   <si>
@@ -4436,18 +4316,12 @@
     <t xml:space="preserve">-6515.59|83267.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6147.59|82473.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6147.59|82064.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-5990.59|81762.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6371.59|81762.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6530.59|82033.08|77527.95</t>
   </si>
   <si>
@@ -4457,9 +4331,6 @@
     <t xml:space="preserve">-7087.59|82473.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7087.59|82064.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6930.59|81762.08|77527.95</t>
   </si>
   <si>
@@ -4472,9 +4343,6 @@
     <t xml:space="preserve">-6925.59|82303.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8066.59|82473.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7770.59|82064.08|77527.95</t>
   </si>
   <si>
@@ -4487,9 +4355,6 @@
     <t xml:space="preserve">-8324.59|82303.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7904.59|82303.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7850.59|81249.08|77527.95</t>
   </si>
   <si>
@@ -4502,9 +4367,6 @@
     <t xml:space="preserve">-8108.59|81488.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-7688.59|81488.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6893.59|81249.08|77527.95</t>
   </si>
   <si>
@@ -4517,9 +4379,6 @@
     <t xml:space="preserve">-7151.59|81488.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6731.59|81488.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6164.59|80645.08|77613.95</t>
   </si>
   <si>
@@ -4529,18 +4388,12 @@
     <t xml:space="preserve">-6164.59|81453.08|77613.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6007.59|80343.08|77613.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-6388.59|80343.08|77613.95</t>
   </si>
   <si>
     <t xml:space="preserve">-6547.59|80614.08|77613.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-6002.59|80884.08|77613.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-10032.59|80947.08|77527.95</t>
   </si>
   <si>
@@ -4553,9 +4406,6 @@
     <t xml:space="preserve">-8851.59|81249.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8555.59|81249.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-10289.59|82192.08|77527.95</t>
   </si>
   <si>
@@ -4565,9 +4415,6 @@
     <t xml:space="preserve">-10323.59|82733.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-9903.59|83115.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-9773.59|83632.08|77527.95</t>
   </si>
   <si>
@@ -4580,9 +4427,6 @@
     <t xml:space="preserve">-9378.59|82619.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8911.59|82844.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-8812.59|82494.08|77527.95</t>
   </si>
   <si>
@@ -4592,18 +4436,12 @@
     <t xml:space="preserve">-10362.59|83340.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-10521.59|83611.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-10396.59|83881.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-9926.59|82421.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-9729.59|81957.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-9556.59|82366.08|77527.95</t>
   </si>
   <si>
@@ -4613,18 +4451,12 @@
     <t xml:space="preserve">-8885.59|83642.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-9024.59|83340.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-9405.59|83340.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-8074.59|80057.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-8233.59|80328.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-7850.59|80359.08|77527.95</t>
   </si>
   <si>
@@ -4640,36 +4472,24 @@
     <t xml:space="preserve">-10891.59|80755.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-10595.59|80755.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-11274.59|80724.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-10734.59|80453.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-11149.59|81849.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-10219.59|81786.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-10931.59|82194.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-10595.59|81610.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-11274.59|81579.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-11115.59|81308.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-9973.59|80101.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-9715.59|79862.08|77527.95</t>
   </si>
   <si>
@@ -4679,9 +4499,6 @@
     <t xml:space="preserve">-9939.59|79560.08|77527.95</t>
   </si>
   <si>
-    <t xml:space="preserve">-9558.59|79560.08|77527.95</t>
-  </si>
-  <si>
     <t xml:space="preserve">-8693.59|79824.08|77527.95</t>
   </si>
   <si>
@@ -4701,9 +4518,6 @@
   </si>
   <si>
     <t xml:space="preserve">-6939.59|79862.08|77527.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6643.59|79862.08|77527.95</t>
   </si>
   <si>
     <t xml:space="preserve">-16357.59|94860.08|93366.95</t>
@@ -5292,10 +5106,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E1860"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1591" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1611" activeCellId="0" sqref="F1611"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1529" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1546" activeCellId="0" sqref="G1546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22363,7 +22177,7 @@
         <v>1398</v>
       </c>
       <c r="C1393" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1394" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22374,7 +22188,7 @@
         <v>1399</v>
       </c>
       <c r="C1394" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1395" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22385,7 +22199,7 @@
         <v>1400</v>
       </c>
       <c r="C1395" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1396" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22396,7 +22210,7 @@
         <v>1401</v>
       </c>
       <c r="C1396" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1397" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22407,7 +22221,7 @@
         <v>1402</v>
       </c>
       <c r="C1397" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1398" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22418,7 +22232,7 @@
         <v>1403</v>
       </c>
       <c r="C1398" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1399" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22429,7 +22243,7 @@
         <v>1404</v>
       </c>
       <c r="C1399" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1400" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22440,7 +22254,7 @@
         <v>1405</v>
       </c>
       <c r="C1400" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1401" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22451,7 +22265,7 @@
         <v>1406</v>
       </c>
       <c r="C1401" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1402" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22462,7 +22276,7 @@
         <v>1407</v>
       </c>
       <c r="C1402" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1403" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22473,7 +22287,7 @@
         <v>1408</v>
       </c>
       <c r="C1403" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1404" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22484,7 +22298,7 @@
         <v>1409</v>
       </c>
       <c r="C1404" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1405" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22495,7 +22309,7 @@
         <v>1410</v>
       </c>
       <c r="C1405" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1406" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22506,7 +22320,7 @@
         <v>1411</v>
       </c>
       <c r="C1406" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1407" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22517,7 +22331,7 @@
         <v>1412</v>
       </c>
       <c r="C1407" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1408" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22528,7 +22342,7 @@
         <v>1413</v>
       </c>
       <c r="C1408" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1409" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22539,7 +22353,7 @@
         <v>1414</v>
       </c>
       <c r="C1409" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1410" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22550,7 +22364,7 @@
         <v>1415</v>
       </c>
       <c r="C1410" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1411" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22561,7 +22375,7 @@
         <v>1416</v>
       </c>
       <c r="C1411" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1412" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22572,7 +22386,7 @@
         <v>1417</v>
       </c>
       <c r="C1412" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1413" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22583,7 +22397,7 @@
         <v>1418</v>
       </c>
       <c r="C1413" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1414" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22594,7 +22408,7 @@
         <v>1419</v>
       </c>
       <c r="C1414" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1415" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22605,7 +22419,7 @@
         <v>1420</v>
       </c>
       <c r="C1415" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1416" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22616,7 +22430,7 @@
         <v>1421</v>
       </c>
       <c r="C1416" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1417" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22627,7 +22441,7 @@
         <v>1422</v>
       </c>
       <c r="C1417" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1418" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22638,7 +22452,7 @@
         <v>1423</v>
       </c>
       <c r="C1418" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1419" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22649,7 +22463,7 @@
         <v>1424</v>
       </c>
       <c r="C1419" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1420" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22660,7 +22474,7 @@
         <v>1425</v>
       </c>
       <c r="C1420" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1421" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22671,7 +22485,7 @@
         <v>1426</v>
       </c>
       <c r="C1421" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1422" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22682,7 +22496,7 @@
         <v>1427</v>
       </c>
       <c r="C1422" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1423" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22693,7 +22507,7 @@
         <v>1428</v>
       </c>
       <c r="C1423" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1424" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22704,7 +22518,7 @@
         <v>1429</v>
       </c>
       <c r="C1424" s="3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="1425" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22971,7 +22785,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="1449" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1449" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1449" s="3" t="n">
         <v>1445</v>
       </c>
@@ -23408,7 +23222,7 @@
         <v>1493</v>
       </c>
       <c r="C1488" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1489" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23419,7 +23233,7 @@
         <v>1494</v>
       </c>
       <c r="C1489" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1490" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23430,7 +23244,7 @@
         <v>1495</v>
       </c>
       <c r="C1490" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1491" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23441,7 +23255,7 @@
         <v>1496</v>
       </c>
       <c r="C1491" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1492" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23452,7 +23266,7 @@
         <v>1497</v>
       </c>
       <c r="C1492" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1493" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23463,7 +23277,7 @@
         <v>1498</v>
       </c>
       <c r="C1493" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1494" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23474,7 +23288,7 @@
         <v>1499</v>
       </c>
       <c r="C1494" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1495" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23485,7 +23299,7 @@
         <v>1500</v>
       </c>
       <c r="C1495" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1496" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23496,7 +23310,7 @@
         <v>1501</v>
       </c>
       <c r="C1496" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1497" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23507,7 +23321,7 @@
         <v>1502</v>
       </c>
       <c r="C1497" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1498" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23518,7 +23332,7 @@
         <v>1503</v>
       </c>
       <c r="C1498" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1499" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23529,7 +23343,7 @@
         <v>1504</v>
       </c>
       <c r="C1499" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1500" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23540,7 +23354,7 @@
         <v>1505</v>
       </c>
       <c r="C1500" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1501" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23551,7 +23365,7 @@
         <v>1506</v>
       </c>
       <c r="C1501" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1502" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23562,7 +23376,7 @@
         <v>1507</v>
       </c>
       <c r="C1502" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1503" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23573,7 +23387,7 @@
         <v>1508</v>
       </c>
       <c r="C1503" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1504" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23584,7 +23398,7 @@
         <v>1509</v>
       </c>
       <c r="C1504" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1505" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23595,7 +23409,7 @@
         <v>1510</v>
       </c>
       <c r="C1505" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1506" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23606,7 +23420,7 @@
         <v>1511</v>
       </c>
       <c r="C1506" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1507" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23617,7 +23431,7 @@
         <v>1512</v>
       </c>
       <c r="C1507" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1508" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23628,7 +23442,7 @@
         <v>1513</v>
       </c>
       <c r="C1508" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1509" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23639,7 +23453,7 @@
         <v>1514</v>
       </c>
       <c r="C1509" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1510" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23650,7 +23464,7 @@
         <v>1515</v>
       </c>
       <c r="C1510" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1511" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23661,7 +23475,7 @@
         <v>1516</v>
       </c>
       <c r="C1511" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1512" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23672,7 +23486,7 @@
         <v>1517</v>
       </c>
       <c r="C1512" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1513" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23683,7 +23497,7 @@
         <v>1518</v>
       </c>
       <c r="C1513" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1514" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23694,7 +23508,7 @@
         <v>1519</v>
       </c>
       <c r="C1514" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1515" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23705,7 +23519,7 @@
         <v>1520</v>
       </c>
       <c r="C1515" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1516" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23716,7 +23530,7 @@
         <v>1521</v>
       </c>
       <c r="C1516" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1517" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23727,7 +23541,7 @@
         <v>1522</v>
       </c>
       <c r="C1517" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1518" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23738,7 +23552,7 @@
         <v>1523</v>
       </c>
       <c r="C1518" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1519" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23749,7 +23563,7 @@
         <v>1524</v>
       </c>
       <c r="C1519" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1520" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23760,7 +23574,7 @@
         <v>1525</v>
       </c>
       <c r="C1520" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1521" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23771,7 +23585,7 @@
         <v>1526</v>
       </c>
       <c r="C1521" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1522" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23782,7 +23596,7 @@
         <v>1527</v>
       </c>
       <c r="C1522" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1523" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23793,7 +23607,7 @@
         <v>1528</v>
       </c>
       <c r="C1523" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1524" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23804,7 +23618,7 @@
         <v>1529</v>
       </c>
       <c r="C1524" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1525" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23815,7 +23629,7 @@
         <v>1530</v>
       </c>
       <c r="C1525" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1526" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23826,7 +23640,7 @@
         <v>1531</v>
       </c>
       <c r="C1526" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1527" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23837,7 +23651,7 @@
         <v>1532</v>
       </c>
       <c r="C1527" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1528" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23848,7 +23662,7 @@
         <v>1533</v>
       </c>
       <c r="C1528" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1529" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23859,7 +23673,7 @@
         <v>1534</v>
       </c>
       <c r="C1529" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1530" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23870,7 +23684,7 @@
         <v>1535</v>
       </c>
       <c r="C1530" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1531" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23881,7 +23695,7 @@
         <v>1536</v>
       </c>
       <c r="C1531" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1532" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23892,7 +23706,7 @@
         <v>1537</v>
       </c>
       <c r="C1532" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1533" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23903,7 +23717,7 @@
         <v>1538</v>
       </c>
       <c r="C1533" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1534" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23914,7 +23728,7 @@
         <v>1539</v>
       </c>
       <c r="C1534" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1535" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23925,7 +23739,7 @@
         <v>1540</v>
       </c>
       <c r="C1535" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1536" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23936,7 +23750,7 @@
         <v>1541</v>
       </c>
       <c r="C1536" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1537" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23947,7 +23761,7 @@
         <v>1542</v>
       </c>
       <c r="C1537" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1538" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23958,7 +23772,7 @@
         <v>1543</v>
       </c>
       <c r="C1538" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1539" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23969,7 +23783,7 @@
         <v>1544</v>
       </c>
       <c r="C1539" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1540" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23980,7 +23794,7 @@
         <v>1545</v>
       </c>
       <c r="C1540" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1541" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23991,7 +23805,7 @@
         <v>1546</v>
       </c>
       <c r="C1541" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1542" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24002,7 +23816,7 @@
         <v>1547</v>
       </c>
       <c r="C1542" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1543" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24013,7 +23827,7 @@
         <v>1548</v>
       </c>
       <c r="C1543" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1544" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24024,746 +23838,374 @@
         <v>1549</v>
       </c>
       <c r="C1544" s="3" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1545" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1545" s="3" t="n">
         <v>1541</v>
       </c>
-      <c r="B1545" s="13" t="s">
+      <c r="B1545" s="14" t="s">
         <v>1550</v>
       </c>
-      <c r="C1545" s="3" t="n">
-        <v>2008</v>
+      <c r="C1545" s="15" t="n">
+        <v>2007</v>
+      </c>
+      <c r="D1545" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1546" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1546" s="3" t="n">
         <v>1542</v>
       </c>
-      <c r="B1546" s="13" t="s">
+      <c r="B1546" s="14" t="s">
         <v>1551</v>
       </c>
-      <c r="C1546" s="3" t="n">
+      <c r="C1546" s="15" t="n">
         <v>2008</v>
+      </c>
+      <c r="D1546" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1547" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1547" s="3" t="n">
         <v>1543</v>
       </c>
-      <c r="B1547" s="13" t="s">
+      <c r="B1547" s="14" t="s">
         <v>1552</v>
       </c>
-      <c r="C1547" s="3" t="n">
-        <v>2008</v>
+      <c r="C1547" s="15" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D1547" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1548" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1548" s="3" t="n">
         <v>1544</v>
       </c>
-      <c r="B1548" s="13" t="s">
+      <c r="B1548" s="14" t="s">
         <v>1553</v>
       </c>
-      <c r="C1548" s="3" t="n">
-        <v>2008</v>
+      <c r="C1548" s="15" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D1548" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="1549" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1549" s="3" t="n">
-        <v>1545</v>
-      </c>
-      <c r="B1549" s="13" t="s">
-        <v>1554</v>
-      </c>
-      <c r="C1549" s="3" t="n">
-        <v>2008</v>
-      </c>
+      <c r="A1549" s="3"/>
+      <c r="B1549" s="3"/>
+      <c r="C1549" s="3"/>
     </row>
     <row r="1550" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1550" s="3" t="n">
-        <v>1546</v>
-      </c>
-      <c r="B1550" s="13" t="s">
-        <v>1555</v>
-      </c>
-      <c r="C1550" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1550" s="3"/>
+      <c r="B1550" s="3"/>
+      <c r="C1550" s="3"/>
     </row>
     <row r="1551" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1551" s="3" t="n">
-        <v>1547</v>
-      </c>
-      <c r="B1551" s="13" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C1551" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1551" s="3"/>
+      <c r="B1551" s="3"/>
+      <c r="C1551" s="3"/>
     </row>
     <row r="1552" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1552" s="3" t="n">
-        <v>1548</v>
-      </c>
-      <c r="B1552" s="13" t="s">
-        <v>1557</v>
-      </c>
-      <c r="C1552" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1552" s="3"/>
+      <c r="B1552" s="3"/>
+      <c r="C1552" s="3"/>
     </row>
     <row r="1553" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1553" s="3" t="n">
-        <v>1549</v>
-      </c>
-      <c r="B1553" s="13" t="s">
-        <v>1558</v>
-      </c>
-      <c r="C1553" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1553" s="3"/>
+      <c r="B1553" s="3"/>
+      <c r="C1553" s="3"/>
     </row>
     <row r="1554" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1554" s="3" t="n">
-        <v>1550</v>
-      </c>
-      <c r="B1554" s="13" t="s">
-        <v>1559</v>
-      </c>
-      <c r="C1554" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1554" s="3"/>
+      <c r="B1554" s="3"/>
+      <c r="C1554" s="3"/>
     </row>
     <row r="1555" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1555" s="3" t="n">
-        <v>1551</v>
-      </c>
-      <c r="B1555" s="13" t="s">
-        <v>1560</v>
-      </c>
-      <c r="C1555" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1555" s="3"/>
+      <c r="B1555" s="3"/>
+      <c r="C1555" s="3"/>
     </row>
     <row r="1556" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1556" s="3" t="n">
-        <v>1552</v>
-      </c>
-      <c r="B1556" s="13" t="s">
-        <v>1561</v>
-      </c>
-      <c r="C1556" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1556" s="3"/>
+      <c r="B1556" s="3"/>
+      <c r="C1556" s="3"/>
     </row>
     <row r="1557" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1557" s="3" t="n">
-        <v>1553</v>
-      </c>
-      <c r="B1557" s="13" t="s">
-        <v>1562</v>
-      </c>
-      <c r="C1557" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1557" s="3"/>
+      <c r="B1557" s="3"/>
+      <c r="C1557" s="3"/>
     </row>
     <row r="1558" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1558" s="3" t="n">
-        <v>1554</v>
-      </c>
-      <c r="B1558" s="13" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C1558" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1558" s="3"/>
+      <c r="B1558" s="3"/>
+      <c r="C1558" s="3"/>
     </row>
     <row r="1559" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1559" s="3" t="n">
-        <v>1555</v>
-      </c>
-      <c r="B1559" s="13" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C1559" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1559" s="3"/>
+      <c r="B1559" s="3"/>
+      <c r="C1559" s="3"/>
     </row>
     <row r="1560" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1560" s="3" t="n">
-        <v>1556</v>
-      </c>
-      <c r="B1560" s="13" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C1560" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1560" s="3"/>
+      <c r="B1560" s="3"/>
+      <c r="C1560" s="3"/>
     </row>
     <row r="1561" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1561" s="3" t="n">
-        <v>1557</v>
-      </c>
-      <c r="B1561" s="13" t="s">
-        <v>1566</v>
-      </c>
-      <c r="C1561" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1561" s="3"/>
+      <c r="B1561" s="3"/>
+      <c r="C1561" s="3"/>
     </row>
     <row r="1562" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1562" s="3" t="n">
-        <v>1558</v>
-      </c>
-      <c r="B1562" s="13" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C1562" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1562" s="3"/>
+      <c r="B1562" s="3"/>
+      <c r="C1562" s="3"/>
     </row>
     <row r="1563" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1563" s="3" t="n">
-        <v>1559</v>
-      </c>
-      <c r="B1563" s="13" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C1563" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1563" s="3"/>
+      <c r="B1563" s="3"/>
+      <c r="C1563" s="3"/>
     </row>
     <row r="1564" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1564" s="3" t="n">
-        <v>1560</v>
-      </c>
-      <c r="B1564" s="13" t="s">
-        <v>1569</v>
-      </c>
-      <c r="C1564" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1564" s="3"/>
+      <c r="B1564" s="3"/>
+      <c r="C1564" s="3"/>
     </row>
     <row r="1565" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1565" s="3" t="n">
-        <v>1561</v>
-      </c>
-      <c r="B1565" s="13" t="s">
-        <v>1570</v>
-      </c>
-      <c r="C1565" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1565" s="3"/>
+      <c r="B1565" s="3"/>
+      <c r="C1565" s="3"/>
     </row>
     <row r="1566" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1566" s="3" t="n">
-        <v>1562</v>
-      </c>
-      <c r="B1566" s="13" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C1566" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1566" s="3"/>
+      <c r="B1566" s="3"/>
+      <c r="C1566" s="3"/>
     </row>
     <row r="1567" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1567" s="3" t="n">
-        <v>1563</v>
-      </c>
-      <c r="B1567" s="13" t="s">
-        <v>1572</v>
-      </c>
-      <c r="C1567" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1567" s="3"/>
+      <c r="B1567" s="3"/>
+      <c r="C1567" s="3"/>
     </row>
     <row r="1568" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1568" s="3" t="n">
-        <v>1564</v>
-      </c>
-      <c r="B1568" s="13" t="s">
-        <v>1573</v>
-      </c>
-      <c r="C1568" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1568" s="3"/>
+      <c r="B1568" s="3"/>
+      <c r="C1568" s="3"/>
     </row>
     <row r="1569" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1569" s="3" t="n">
-        <v>1565</v>
-      </c>
-      <c r="B1569" s="13" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C1569" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1569" s="3"/>
+      <c r="B1569" s="3"/>
+      <c r="C1569" s="3"/>
     </row>
     <row r="1570" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1570" s="3" t="n">
-        <v>1566</v>
-      </c>
-      <c r="B1570" s="13" t="s">
-        <v>1575</v>
-      </c>
-      <c r="C1570" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1570" s="3"/>
+      <c r="B1570" s="3"/>
+      <c r="C1570" s="3"/>
     </row>
     <row r="1571" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1571" s="3" t="n">
-        <v>1567</v>
-      </c>
-      <c r="B1571" s="13" t="s">
-        <v>1576</v>
-      </c>
-      <c r="C1571" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1571" s="3"/>
+      <c r="B1571" s="3"/>
+      <c r="C1571" s="3"/>
     </row>
     <row r="1572" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1572" s="3" t="n">
-        <v>1568</v>
-      </c>
-      <c r="B1572" s="13" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C1572" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1572" s="3"/>
+      <c r="B1572" s="3"/>
+      <c r="C1572" s="3"/>
     </row>
     <row r="1573" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1573" s="3" t="n">
-        <v>1569</v>
-      </c>
-      <c r="B1573" s="13" t="s">
-        <v>1578</v>
-      </c>
-      <c r="C1573" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1573" s="3"/>
+      <c r="B1573" s="3"/>
+      <c r="C1573" s="3"/>
     </row>
     <row r="1574" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1574" s="3" t="n">
-        <v>1570</v>
-      </c>
-      <c r="B1574" s="13" t="s">
-        <v>1579</v>
-      </c>
-      <c r="C1574" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1574" s="3"/>
+      <c r="B1574" s="3"/>
+      <c r="C1574" s="3"/>
     </row>
     <row r="1575" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1575" s="3" t="n">
-        <v>1571</v>
-      </c>
-      <c r="B1575" s="13" t="s">
-        <v>1580</v>
-      </c>
-      <c r="C1575" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1575" s="3"/>
+      <c r="B1575" s="3"/>
+      <c r="C1575" s="3"/>
     </row>
     <row r="1576" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1576" s="3" t="n">
-        <v>1572</v>
-      </c>
-      <c r="B1576" s="13" t="s">
-        <v>1581</v>
-      </c>
-      <c r="C1576" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1576" s="3"/>
+      <c r="B1576" s="3"/>
+      <c r="C1576" s="3"/>
     </row>
     <row r="1577" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1577" s="3" t="n">
-        <v>1573</v>
-      </c>
-      <c r="B1577" s="13" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C1577" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1577" s="3"/>
+      <c r="B1577" s="3"/>
+      <c r="C1577" s="3"/>
     </row>
     <row r="1578" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1578" s="3" t="n">
-        <v>1574</v>
-      </c>
-      <c r="B1578" s="13" t="s">
-        <v>1583</v>
-      </c>
-      <c r="C1578" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1578" s="3"/>
+      <c r="B1578" s="3"/>
+      <c r="C1578" s="3"/>
     </row>
     <row r="1579" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1579" s="3" t="n">
-        <v>1575</v>
-      </c>
-      <c r="B1579" s="13" t="s">
-        <v>1584</v>
-      </c>
-      <c r="C1579" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1579" s="3"/>
+      <c r="B1579" s="3"/>
+      <c r="C1579" s="3"/>
     </row>
     <row r="1580" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1580" s="3" t="n">
-        <v>1576</v>
-      </c>
-      <c r="B1580" s="13" t="s">
-        <v>1585</v>
-      </c>
-      <c r="C1580" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1580" s="3"/>
+      <c r="B1580" s="3"/>
+      <c r="C1580" s="3"/>
     </row>
     <row r="1581" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1581" s="3" t="n">
-        <v>1577</v>
-      </c>
-      <c r="B1581" s="13" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C1581" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1581" s="3"/>
+      <c r="B1581" s="3"/>
+      <c r="C1581" s="3"/>
     </row>
     <row r="1582" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1582" s="3" t="n">
-        <v>1578</v>
-      </c>
-      <c r="B1582" s="13" t="s">
-        <v>1587</v>
-      </c>
-      <c r="C1582" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1582" s="3"/>
+      <c r="B1582" s="3"/>
+      <c r="C1582" s="3"/>
     </row>
     <row r="1583" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1583" s="3" t="n">
-        <v>1579</v>
-      </c>
-      <c r="B1583" s="13" t="s">
-        <v>1588</v>
-      </c>
-      <c r="C1583" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1583" s="3"/>
+      <c r="B1583" s="3"/>
+      <c r="C1583" s="3"/>
     </row>
     <row r="1584" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1584" s="3" t="n">
-        <v>1580</v>
-      </c>
-      <c r="B1584" s="13" t="s">
-        <v>1589</v>
-      </c>
-      <c r="C1584" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1584" s="3"/>
+      <c r="B1584" s="3"/>
+      <c r="C1584" s="3"/>
     </row>
     <row r="1585" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1585" s="3" t="n">
-        <v>1581</v>
-      </c>
-      <c r="B1585" s="13" t="s">
-        <v>1590</v>
-      </c>
-      <c r="C1585" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1585" s="3"/>
+      <c r="B1585" s="3"/>
+      <c r="C1585" s="3"/>
     </row>
     <row r="1586" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1586" s="3" t="n">
-        <v>1582</v>
-      </c>
-      <c r="B1586" s="13" t="s">
-        <v>1591</v>
-      </c>
-      <c r="C1586" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1586" s="3"/>
+      <c r="B1586" s="3"/>
+      <c r="C1586" s="3"/>
     </row>
     <row r="1587" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1587" s="3" t="n">
-        <v>1583</v>
-      </c>
-      <c r="B1587" s="13" t="s">
-        <v>1592</v>
-      </c>
-      <c r="C1587" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1587" s="3"/>
+      <c r="B1587" s="3"/>
+      <c r="C1587" s="3"/>
     </row>
     <row r="1588" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1588" s="3" t="n">
-        <v>1584</v>
-      </c>
-      <c r="B1588" s="13" t="s">
-        <v>1593</v>
-      </c>
-      <c r="C1588" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1588" s="3"/>
+      <c r="B1588" s="3"/>
+      <c r="C1588" s="3"/>
     </row>
     <row r="1589" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1589" s="3" t="n">
-        <v>1585</v>
-      </c>
-      <c r="B1589" s="13" t="s">
-        <v>1594</v>
-      </c>
-      <c r="C1589" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1589" s="3"/>
+      <c r="B1589" s="3"/>
+      <c r="C1589" s="3"/>
     </row>
     <row r="1590" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1590" s="3" t="n">
-        <v>1586</v>
-      </c>
-      <c r="B1590" s="13" t="s">
-        <v>1595</v>
-      </c>
-      <c r="C1590" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1590" s="3"/>
+      <c r="B1590" s="3"/>
+      <c r="C1590" s="3"/>
     </row>
     <row r="1591" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1591" s="3" t="n">
-        <v>1587</v>
-      </c>
-      <c r="B1591" s="13" t="s">
-        <v>1596</v>
-      </c>
-      <c r="C1591" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1591" s="3"/>
+      <c r="B1591" s="3"/>
+      <c r="C1591" s="3"/>
     </row>
     <row r="1592" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1592" s="3" t="n">
-        <v>1588</v>
-      </c>
-      <c r="B1592" s="13" t="s">
-        <v>1597</v>
-      </c>
-      <c r="C1592" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1592" s="3"/>
+      <c r="B1592" s="3"/>
+      <c r="C1592" s="3"/>
     </row>
     <row r="1593" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1593" s="3" t="n">
-        <v>1589</v>
-      </c>
-      <c r="B1593" s="13" t="s">
-        <v>1598</v>
-      </c>
-      <c r="C1593" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1593" s="3"/>
+      <c r="B1593" s="3"/>
+      <c r="C1593" s="3"/>
     </row>
     <row r="1594" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1594" s="3" t="n">
-        <v>1590</v>
-      </c>
-      <c r="B1594" s="13" t="s">
-        <v>1599</v>
-      </c>
-      <c r="C1594" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1594" s="3"/>
+      <c r="B1594" s="3"/>
+      <c r="C1594" s="3"/>
     </row>
     <row r="1595" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1595" s="3" t="n">
-        <v>1591</v>
-      </c>
-      <c r="B1595" s="13" t="s">
-        <v>1600</v>
-      </c>
-      <c r="C1595" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1595" s="3"/>
+      <c r="B1595" s="3"/>
+      <c r="C1595" s="3"/>
     </row>
     <row r="1596" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1596" s="3" t="n">
-        <v>1592</v>
-      </c>
-      <c r="B1596" s="13" t="s">
-        <v>1601</v>
-      </c>
-      <c r="C1596" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1596" s="3"/>
+      <c r="B1596" s="3"/>
+      <c r="C1596" s="3"/>
     </row>
     <row r="1597" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1597" s="3" t="n">
-        <v>1593</v>
-      </c>
-      <c r="B1597" s="13" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C1597" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1597" s="3"/>
+      <c r="B1597" s="3"/>
+      <c r="C1597" s="3"/>
     </row>
     <row r="1598" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1598" s="3" t="n">
-        <v>1594</v>
-      </c>
-      <c r="B1598" s="13" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C1598" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1598" s="3"/>
+      <c r="B1598" s="3"/>
+      <c r="C1598" s="3"/>
     </row>
     <row r="1599" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1599" s="3" t="n">
-        <v>1595</v>
-      </c>
-      <c r="B1599" s="13" t="s">
-        <v>1604</v>
-      </c>
-      <c r="C1599" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1599" s="3"/>
+      <c r="B1599" s="3"/>
+      <c r="C1599" s="3"/>
     </row>
     <row r="1600" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1600" s="3" t="n">
-        <v>1596</v>
-      </c>
-      <c r="B1600" s="13" t="s">
-        <v>1605</v>
-      </c>
-      <c r="C1600" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1600" s="3"/>
+      <c r="B1600" s="3"/>
+      <c r="C1600" s="3"/>
     </row>
     <row r="1601" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1601" s="3" t="n">
-        <v>1597</v>
-      </c>
-      <c r="B1601" s="13" t="s">
-        <v>1606</v>
-      </c>
-      <c r="C1601" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1601" s="3"/>
+      <c r="B1601" s="3"/>
+      <c r="C1601" s="3"/>
     </row>
     <row r="1602" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1602" s="3" t="n">
-        <v>1598</v>
-      </c>
-      <c r="B1602" s="13" t="s">
-        <v>1607</v>
-      </c>
-      <c r="C1602" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1602" s="3"/>
+      <c r="B1602" s="3"/>
+      <c r="C1602" s="3"/>
     </row>
     <row r="1603" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1603" s="3" t="n">
-        <v>1599</v>
-      </c>
-      <c r="B1603" s="13" t="s">
-        <v>1608</v>
-      </c>
-      <c r="C1603" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1603" s="3"/>
+      <c r="B1603" s="3"/>
+      <c r="C1603" s="3"/>
     </row>
     <row r="1604" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1604" s="3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="B1604" s="13" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C1604" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1604" s="3"/>
+      <c r="B1604" s="3"/>
+      <c r="C1604" s="3"/>
     </row>
     <row r="1605" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1605" s="3" t="n">
-        <v>1601</v>
-      </c>
-      <c r="B1605" s="13" t="s">
-        <v>1610</v>
-      </c>
-      <c r="C1605" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1605" s="3"/>
+      <c r="B1605" s="3"/>
+      <c r="C1605" s="3"/>
     </row>
     <row r="1606" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1606" s="3" t="n">
-        <v>1602</v>
-      </c>
-      <c r="B1606" s="13" t="s">
-        <v>1611</v>
-      </c>
-      <c r="C1606" s="3" t="n">
-        <v>2009</v>
-      </c>
+      <c r="A1606" s="3"/>
+      <c r="B1606" s="3"/>
+      <c r="C1606" s="3"/>
     </row>
     <row r="1607" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1607" s="3" t="n">
-        <v>1603</v>
-      </c>
-      <c r="B1607" s="14" t="s">
-        <v>1612</v>
-      </c>
-      <c r="C1607" s="15" t="n">
-        <v>2007</v>
-      </c>
-      <c r="D1607" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A1607" s="3"/>
+      <c r="B1607" s="3"/>
+      <c r="C1607" s="3"/>
     </row>
     <row r="1608" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1608" s="3" t="n">
-        <v>1604</v>
-      </c>
-      <c r="B1608" s="14" t="s">
-        <v>1613</v>
-      </c>
-      <c r="C1608" s="15" t="n">
-        <v>2008</v>
-      </c>
-      <c r="D1608" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A1608" s="3"/>
+      <c r="B1608" s="3"/>
+      <c r="C1608" s="3"/>
     </row>
     <row r="1609" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1609" s="3" t="n">
-        <v>1605</v>
-      </c>
-      <c r="B1609" s="14" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C1609" s="15" t="n">
-        <v>2009</v>
-      </c>
-      <c r="D1609" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A1609" s="3"/>
+      <c r="B1609" s="3"/>
+      <c r="C1609" s="3"/>
     </row>
     <row r="1610" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1610" s="3" t="n">
-        <v>1606</v>
-      </c>
-      <c r="B1610" s="14" t="s">
-        <v>1615</v>
-      </c>
-      <c r="C1610" s="15" t="n">
-        <v>2010</v>
-      </c>
-      <c r="D1610" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A1610" s="3"/>
+      <c r="B1610" s="3"/>
+      <c r="C1610" s="3"/>
     </row>
     <row r="1611" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1611" s="3"/>
@@ -26015,318 +25457,6 @@
       <c r="B1860" s="3"/>
       <c r="C1860" s="3"/>
     </row>
-    <row r="1861" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1861" s="3"/>
-      <c r="B1861" s="3"/>
-      <c r="C1861" s="3"/>
-    </row>
-    <row r="1862" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1862" s="3"/>
-      <c r="B1862" s="3"/>
-      <c r="C1862" s="3"/>
-    </row>
-    <row r="1863" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1863" s="3"/>
-      <c r="B1863" s="3"/>
-      <c r="C1863" s="3"/>
-    </row>
-    <row r="1864" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1864" s="3"/>
-      <c r="B1864" s="3"/>
-      <c r="C1864" s="3"/>
-    </row>
-    <row r="1865" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1865" s="3"/>
-      <c r="B1865" s="3"/>
-      <c r="C1865" s="3"/>
-    </row>
-    <row r="1866" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1866" s="3"/>
-      <c r="B1866" s="3"/>
-      <c r="C1866" s="3"/>
-    </row>
-    <row r="1867" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1867" s="3"/>
-      <c r="B1867" s="3"/>
-      <c r="C1867" s="3"/>
-    </row>
-    <row r="1868" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1868" s="3"/>
-      <c r="B1868" s="3"/>
-      <c r="C1868" s="3"/>
-    </row>
-    <row r="1869" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1869" s="3"/>
-      <c r="B1869" s="3"/>
-      <c r="C1869" s="3"/>
-    </row>
-    <row r="1870" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1870" s="3"/>
-      <c r="B1870" s="3"/>
-      <c r="C1870" s="3"/>
-    </row>
-    <row r="1871" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1871" s="3"/>
-      <c r="B1871" s="3"/>
-      <c r="C1871" s="3"/>
-    </row>
-    <row r="1872" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1872" s="3"/>
-      <c r="B1872" s="3"/>
-      <c r="C1872" s="3"/>
-    </row>
-    <row r="1873" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1873" s="3"/>
-      <c r="B1873" s="3"/>
-      <c r="C1873" s="3"/>
-    </row>
-    <row r="1874" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1874" s="3"/>
-      <c r="B1874" s="3"/>
-      <c r="C1874" s="3"/>
-    </row>
-    <row r="1875" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1875" s="3"/>
-      <c r="B1875" s="3"/>
-      <c r="C1875" s="3"/>
-    </row>
-    <row r="1876" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1876" s="3"/>
-      <c r="B1876" s="3"/>
-      <c r="C1876" s="3"/>
-    </row>
-    <row r="1877" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1877" s="3"/>
-      <c r="B1877" s="3"/>
-      <c r="C1877" s="3"/>
-    </row>
-    <row r="1878" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1878" s="3"/>
-      <c r="B1878" s="3"/>
-      <c r="C1878" s="3"/>
-    </row>
-    <row r="1879" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1879" s="3"/>
-      <c r="B1879" s="3"/>
-      <c r="C1879" s="3"/>
-    </row>
-    <row r="1880" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1880" s="3"/>
-      <c r="B1880" s="3"/>
-      <c r="C1880" s="3"/>
-    </row>
-    <row r="1881" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1881" s="3"/>
-      <c r="B1881" s="3"/>
-      <c r="C1881" s="3"/>
-    </row>
-    <row r="1882" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1882" s="3"/>
-      <c r="B1882" s="3"/>
-      <c r="C1882" s="3"/>
-    </row>
-    <row r="1883" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1883" s="3"/>
-      <c r="B1883" s="3"/>
-      <c r="C1883" s="3"/>
-    </row>
-    <row r="1884" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1884" s="3"/>
-      <c r="B1884" s="3"/>
-      <c r="C1884" s="3"/>
-    </row>
-    <row r="1885" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1885" s="3"/>
-      <c r="B1885" s="3"/>
-      <c r="C1885" s="3"/>
-    </row>
-    <row r="1886" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1886" s="3"/>
-      <c r="B1886" s="3"/>
-      <c r="C1886" s="3"/>
-    </row>
-    <row r="1887" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1887" s="3"/>
-      <c r="B1887" s="3"/>
-      <c r="C1887" s="3"/>
-    </row>
-    <row r="1888" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1888" s="3"/>
-      <c r="B1888" s="3"/>
-      <c r="C1888" s="3"/>
-    </row>
-    <row r="1889" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1889" s="3"/>
-      <c r="B1889" s="3"/>
-      <c r="C1889" s="3"/>
-    </row>
-    <row r="1890" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1890" s="3"/>
-      <c r="B1890" s="3"/>
-      <c r="C1890" s="3"/>
-    </row>
-    <row r="1891" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1891" s="3"/>
-      <c r="B1891" s="3"/>
-      <c r="C1891" s="3"/>
-    </row>
-    <row r="1892" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1892" s="3"/>
-      <c r="B1892" s="3"/>
-      <c r="C1892" s="3"/>
-    </row>
-    <row r="1893" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1893" s="3"/>
-      <c r="B1893" s="3"/>
-      <c r="C1893" s="3"/>
-    </row>
-    <row r="1894" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1894" s="3"/>
-      <c r="B1894" s="3"/>
-      <c r="C1894" s="3"/>
-    </row>
-    <row r="1895" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1895" s="3"/>
-      <c r="B1895" s="3"/>
-      <c r="C1895" s="3"/>
-    </row>
-    <row r="1896" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1896" s="3"/>
-      <c r="B1896" s="3"/>
-      <c r="C1896" s="3"/>
-    </row>
-    <row r="1897" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1897" s="3"/>
-      <c r="B1897" s="3"/>
-      <c r="C1897" s="3"/>
-    </row>
-    <row r="1898" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1898" s="3"/>
-      <c r="B1898" s="3"/>
-      <c r="C1898" s="3"/>
-    </row>
-    <row r="1899" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1899" s="3"/>
-      <c r="B1899" s="3"/>
-      <c r="C1899" s="3"/>
-    </row>
-    <row r="1900" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1900" s="3"/>
-      <c r="B1900" s="3"/>
-      <c r="C1900" s="3"/>
-    </row>
-    <row r="1901" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1901" s="3"/>
-      <c r="B1901" s="3"/>
-      <c r="C1901" s="3"/>
-    </row>
-    <row r="1902" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1902" s="3"/>
-      <c r="B1902" s="3"/>
-      <c r="C1902" s="3"/>
-    </row>
-    <row r="1903" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1903" s="3"/>
-      <c r="B1903" s="3"/>
-      <c r="C1903" s="3"/>
-    </row>
-    <row r="1904" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1904" s="3"/>
-      <c r="B1904" s="3"/>
-      <c r="C1904" s="3"/>
-    </row>
-    <row r="1905" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1905" s="3"/>
-      <c r="B1905" s="3"/>
-      <c r="C1905" s="3"/>
-    </row>
-    <row r="1906" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1906" s="3"/>
-      <c r="B1906" s="3"/>
-      <c r="C1906" s="3"/>
-    </row>
-    <row r="1907" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1907" s="3"/>
-      <c r="B1907" s="3"/>
-      <c r="C1907" s="3"/>
-    </row>
-    <row r="1908" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1908" s="3"/>
-      <c r="B1908" s="3"/>
-      <c r="C1908" s="3"/>
-    </row>
-    <row r="1909" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1909" s="3"/>
-      <c r="B1909" s="3"/>
-      <c r="C1909" s="3"/>
-    </row>
-    <row r="1910" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1910" s="3"/>
-      <c r="B1910" s="3"/>
-      <c r="C1910" s="3"/>
-    </row>
-    <row r="1911" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1911" s="3"/>
-      <c r="B1911" s="3"/>
-      <c r="C1911" s="3"/>
-    </row>
-    <row r="1912" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1912" s="3"/>
-      <c r="B1912" s="3"/>
-      <c r="C1912" s="3"/>
-    </row>
-    <row r="1913" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1913" s="3"/>
-      <c r="B1913" s="3"/>
-      <c r="C1913" s="3"/>
-    </row>
-    <row r="1914" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1914" s="3"/>
-      <c r="B1914" s="3"/>
-      <c r="C1914" s="3"/>
-    </row>
-    <row r="1915" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1915" s="3"/>
-      <c r="B1915" s="3"/>
-      <c r="C1915" s="3"/>
-    </row>
-    <row r="1916" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1916" s="3"/>
-      <c r="B1916" s="3"/>
-      <c r="C1916" s="3"/>
-    </row>
-    <row r="1917" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1917" s="3"/>
-      <c r="B1917" s="3"/>
-      <c r="C1917" s="3"/>
-    </row>
-    <row r="1918" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1918" s="3"/>
-      <c r="B1918" s="3"/>
-      <c r="C1918" s="3"/>
-    </row>
-    <row r="1919" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1919" s="3"/>
-      <c r="B1919" s="3"/>
-      <c r="C1919" s="3"/>
-    </row>
-    <row r="1920" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1920" s="3"/>
-      <c r="B1920" s="3"/>
-      <c r="C1920" s="3"/>
-    </row>
-    <row r="1921" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1921" s="3"/>
-      <c r="B1921" s="3"/>
-      <c r="C1921" s="3"/>
-    </row>
-    <row r="1922" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1922" s="3"/>
-      <c r="B1922" s="3"/>
-      <c r="C1922" s="3"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>